<commit_message>
Added power & comms.
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor Tamarin\Documents\GitHub\Canon-Intervalometer\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD63ABD3-5DFF-4434-9793-6A32C9B7083B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8066E066-4B7E-423B-BA1F-AC94A9119E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38295" yWindow="10575" windowWidth="16410" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Part</t>
   </si>
@@ -90,6 +90,48 @@
   </si>
   <si>
     <t>PEC16-4020F-S0024</t>
+  </si>
+  <si>
+    <t>OLED Display</t>
+  </si>
+  <si>
+    <t>Monochroom 0.96" 128x64 OLED grafisch display (kiwi-electronics.com)</t>
+  </si>
+  <si>
+    <t>N-MOSFET</t>
+  </si>
+  <si>
+    <t>BJT</t>
+  </si>
+  <si>
+    <t>USB-C connector</t>
+  </si>
+  <si>
+    <t>U262-161N-4BVC11 XKB Connectivity | C319148 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>DMN2056U-7 Diodes Incorporated | C332302 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>DMN2056U-7</t>
+  </si>
+  <si>
+    <t>SBC847BDW1T1G onsemi | C232475 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>SBC847BDW1T1G</t>
+  </si>
+  <si>
+    <t>U262-161N-4BVC11</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>AZ1117H-3.3TRE1 Diodes Incorporated | C92517 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>AZ1117H-3.3TRE1</t>
   </si>
 </sst>
 </file>
@@ -167,8 +209,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0">
-  <autoFilter ref="A1:F8" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0">
+  <autoFilter ref="A1:F10" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9964CAF8-BC40-4857-A93B-37018EB66BEB}" name="Part"/>
     <tableColumn id="2" xr3:uid="{759936DF-FAE0-45E5-B671-94997451E316}" name="Description"/>
@@ -446,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +501,7 @@
     <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" customWidth="1"/>
+    <col min="6" max="6" width="74.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -567,21 +609,105 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6" s="2">
         <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>23.5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
       <c r="E7" s="2">
         <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>1.24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="E8" s="2">
         <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>0.62</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -590,11 +716,16 @@
     <hyperlink ref="F3" r:id="rId2" display="https://www.lcsc.com/product-detail/Tactile-Switches_TE-Connectivity-4-1437565-2_C86487.html" xr:uid="{B7CBB824-985F-4006-9193-442F3616C6CE}"/>
     <hyperlink ref="F4" r:id="rId3" display="https://www.lcsc.com/product-detail/Audio-Connectors_BOOMELE-Boom-Precision-Elec-C18594_C18594.html" xr:uid="{C1647075-4746-4B4B-BCF9-E4A86FEC0545}"/>
     <hyperlink ref="F5" r:id="rId4" display="https://www.lcsc.com/product-detail/Rotary-Encoders_BOURNS-PEC16-4020F-S0024_C143803.html" xr:uid="{185BFB6A-FB94-49DD-A015-A936F44EFB83}"/>
+    <hyperlink ref="F6" r:id="rId5" display="https://www.kiwi-electronics.com/nl/monochroom-0-96quot-128x64-oled-grafisch-display-754?search=oled" xr:uid="{A3309F31-093D-4FC8-9284-BFB93AB06CD4}"/>
+    <hyperlink ref="F9" r:id="rId6" display="https://www.lcsc.com/product-detail/USB-Connectors_XKB-Connectivity-U262-161N-4BVC11_C319148.html" xr:uid="{26BC4EE9-52FA-4A4D-8B82-8E3B796F58AB}"/>
+    <hyperlink ref="F7" r:id="rId7" display="https://www.lcsc.com/product-detail/MOSFETs_Diodes-Incorporated-DMN2056U-7_C332302.html" xr:uid="{7A4CF6D4-84E8-4D04-82FA-FB06442F1E11}"/>
+    <hyperlink ref="F8" r:id="rId8" display="https://www.lcsc.com/product-detail/Bipolar-Transistors-BJT_onsemi-SBC847BDW1T1G_C232475.html" xr:uid="{4C5F54A5-C086-4BE7-9893-79AB37E3B68C}"/>
+    <hyperlink ref="F10" r:id="rId9" display="https://www.lcsc.com/product-detail/Linear-Voltage-Regulators-LDO_Diodes-Incorporated-AZ1117H-3-3TRE1_C92517.html" xr:uid="{533432A5-B9FC-4EB3-9126-ED23CB9F70D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added missing footprints. First PCB export.
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor Tamarin\Documents\GitHub\Canon-Intervalometer\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CFC205-647D-4057-83B6-3266DD640B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162012F7-DF13-4EF4-9A25-09BFBE70CC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38295" yWindow="10575" windowWidth="16410" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Part</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t>NX3215SA-32.768K-STD-MUA-14 NDK | C156244 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>TC212B106K020Y Sunlord | C177761 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>Tantalum capacitor</t>
+  </si>
+  <si>
+    <t>TAJB226K010RNJ Kyocera AVX | C7198 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>TAJB226K010RNJ</t>
+  </si>
+  <si>
+    <t>TC212B106K020Y</t>
   </si>
 </sst>
 </file>
@@ -218,8 +233,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0">
-  <autoFilter ref="A1:F11" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0">
+  <autoFilter ref="A1:F13" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9964CAF8-BC40-4857-A93B-37018EB66BEB}" name="Part"/>
     <tableColumn id="2" xr3:uid="{759936DF-FAE0-45E5-B671-94997451E316}" name="Description"/>
@@ -497,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,6 +755,48 @@
         <v>34</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.24</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://www.lcsc.com/product-detail/WiFi-Modules_Espressif-Systems-ESP32-PICO-MINI-02-N8R2_C2980306.html" xr:uid="{B458EBDD-0DCE-4A1E-8409-521A960955CA}"/>
@@ -752,11 +809,13 @@
     <hyperlink ref="F8" r:id="rId8" display="https://www.lcsc.com/product-detail/Bipolar-Transistors-BJT_onsemi-SBC847BDW1T1G_C232475.html" xr:uid="{4C5F54A5-C086-4BE7-9893-79AB37E3B68C}"/>
     <hyperlink ref="F10" r:id="rId9" display="https://www.lcsc.com/product-detail/Linear-Voltage-Regulators-LDO_Diodes-Incorporated-AZ1117H-3-3TRE1_C92517.html" xr:uid="{533432A5-B9FC-4EB3-9126-ED23CB9F70D3}"/>
     <hyperlink ref="F11" r:id="rId10" display="https://www.lcsc.com/product-detail/Crystals_NDK-NX3215SA-32-768K-STD-MUA-14_C156244.html" xr:uid="{51CEB293-2ABB-45A6-86DD-E440D74EE607}"/>
+    <hyperlink ref="F12" r:id="rId11" display="https://www.lcsc.com/product-detail/Tantalum-Capacitors_Sunlord-TC212B106K020Y_C177761.html" xr:uid="{8A59700E-4443-423C-BC63-4E003A188415}"/>
+    <hyperlink ref="F13" r:id="rId12" display="https://www.lcsc.com/product-detail/Tantalum-Capacitors_Kyocera-AVX-TAJB226K010RNJ_C7198.html" xr:uid="{22D252D6-E796-4F0A-B86D-ACBDFED42E62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started routing. Added power switch.
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor Tamarin\Documents\GitHub\Canon-Intervalometer\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9087C1E6-5504-433B-8E1E-76D9544B76A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE299A6-BE0E-496C-82C3-3B8111C9CD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38295" yWindow="10575" windowWidth="16410" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Part</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>SIQ-02FVS3</t>
+  </si>
+  <si>
+    <t>MK-12D18-G020 G-Switch | C3019727 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>Slide switch</t>
+  </si>
+  <si>
+    <t>MK-12D18-G020</t>
   </si>
 </sst>
 </file>
@@ -233,8 +242,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0">
-  <autoFilter ref="A1:F13" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0">
+  <autoFilter ref="A1:F14" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9964CAF8-BC40-4857-A93B-37018EB66BEB}" name="Part"/>
     <tableColumn id="2" xr3:uid="{759936DF-FAE0-45E5-B671-94997451E316}" name="Description"/>
@@ -512,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B22" sqref="B21:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,6 +806,27 @@
         <v>35</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.63</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://www.lcsc.com/product-detail/WiFi-Modules_Espressif-Systems-ESP32-PICO-MINI-02-N8R2_C2980306.html" xr:uid="{B458EBDD-0DCE-4A1E-8409-521A960955CA}"/>
@@ -811,11 +841,12 @@
     <hyperlink ref="F12" r:id="rId10" display="https://www.lcsc.com/product-detail/Tantalum-Capacitors_Sunlord-TC212B106K020Y_C177761.html" xr:uid="{8A59700E-4443-423C-BC63-4E003A188415}"/>
     <hyperlink ref="F13" r:id="rId11" display="https://www.lcsc.com/product-detail/Tantalum-Capacitors_Kyocera-AVX-TAJB226K010RNJ_C7198.html" xr:uid="{22D252D6-E796-4F0A-B86D-ACBDFED42E62}"/>
     <hyperlink ref="F5" r:id="rId12" display="https://www.lcsc.com/product-detail/Rotary-Encoders_Mitsumi-Electric-SIQ-02FVS3_C2925423.html" xr:uid="{FB50EC56-7DE9-498C-AAEA-BC393FF7E97F}"/>
+    <hyperlink ref="F14" r:id="rId13" display="https://www.lcsc.com/product-detail/Slide-Switches_G-Switch-MK-12D18-G020_C3019727.html" xr:uid="{E838C8F8-4747-4AE5-B5C6-0AABD0F5FF38}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Routing USB and charger.
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor Tamarin\Documents\GitHub\Canon-Intervalometer\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE299A6-BE0E-496C-82C3-3B8111C9CD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874CCB23-3ECA-43F7-BAF9-D18D16B9393A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38295" yWindow="10575" windowWidth="16410" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Part</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>MK-12D18-G020</t>
+  </si>
+  <si>
+    <t>TP4056 TPOWER | C382139 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>TP4056</t>
+  </si>
+  <si>
+    <t>Charge control circuit</t>
   </si>
 </sst>
 </file>
@@ -242,8 +251,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0">
-  <autoFilter ref="A1:F14" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F15" totalsRowShown="0">
+  <autoFilter ref="A1:F15" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9964CAF8-BC40-4857-A93B-37018EB66BEB}" name="Part"/>
     <tableColumn id="2" xr3:uid="{759936DF-FAE0-45E5-B671-94997451E316}" name="Description"/>
@@ -521,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B21:B22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,6 +836,27 @@
         <v>40</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://www.lcsc.com/product-detail/WiFi-Modules_Espressif-Systems-ESP32-PICO-MINI-02-N8R2_C2980306.html" xr:uid="{B458EBDD-0DCE-4A1E-8409-521A960955CA}"/>
@@ -842,11 +872,12 @@
     <hyperlink ref="F13" r:id="rId11" display="https://www.lcsc.com/product-detail/Tantalum-Capacitors_Kyocera-AVX-TAJB226K010RNJ_C7198.html" xr:uid="{22D252D6-E796-4F0A-B86D-ACBDFED42E62}"/>
     <hyperlink ref="F5" r:id="rId12" display="https://www.lcsc.com/product-detail/Rotary-Encoders_Mitsumi-Electric-SIQ-02FVS3_C2925423.html" xr:uid="{FB50EC56-7DE9-498C-AAEA-BC393FF7E97F}"/>
     <hyperlink ref="F14" r:id="rId13" display="https://www.lcsc.com/product-detail/Slide-Switches_G-Switch-MK-12D18-G020_C3019727.html" xr:uid="{E838C8F8-4747-4AE5-B5C6-0AABD0F5FF38}"/>
+    <hyperlink ref="F15" r:id="rId14" display="https://www.lcsc.com/product-detail/Battery-Management-ICs_TPOWER-TP4056_C382139.html" xr:uid="{111A80ED-4D8C-4F2E-A3B2-170394732200}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>